<commit_message>
Added kangaroo mother care
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_options.xlsx
+++ b/applications/demo/data/national/demo_options.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F96F207E-770F-F64D-8924-EFF69BF38291}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E24F381F-02EB-7942-A1DA-06D2362C8F86}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13020" yWindow="-21140" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs to include" sheetId="3" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="48">
   <si>
     <t>Coverage</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>thrive</t>
+  </si>
+  <si>
+    <t>Kangaroo mother care</t>
   </si>
 </sst>
 </file>
@@ -790,10 +793,10 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -907,65 +910,65 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>4</v>
@@ -973,51 +976,59 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B33" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:B32">
-    <sortCondition ref="A2:A32"/>
+  <sortState ref="A2:B33">
+    <sortCondition ref="A2:A33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1029,10 +1040,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AE33"/>
+  <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1341,7 +1352,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>0</v>
@@ -1358,7 +1369,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>0</v>
@@ -1375,7 +1386,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>0</v>
@@ -1392,7 +1403,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>0</v>
@@ -1409,15 +1420,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="13">
-        <v>0.95</v>
-      </c>
+      <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -1428,13 +1437,15 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
+      <c r="D21" s="13">
+        <v>0.95</v>
+      </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -1445,7 +1456,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>0</v>
@@ -1462,7 +1473,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>0</v>
@@ -1479,15 +1490,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="13"/>
-      <c r="D24" s="13">
-        <v>0.95</v>
-      </c>
+      <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -1498,7 +1507,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>0</v>
@@ -1517,13 +1526,15 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
+      <c r="D26" s="13">
+        <v>0.95</v>
+      </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -1534,7 +1545,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>0</v>
@@ -1551,7 +1562,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>0</v>
@@ -1568,7 +1579,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>0</v>
@@ -1585,7 +1596,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>0</v>
@@ -1602,7 +1613,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>0</v>
@@ -1619,7 +1630,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>0</v>
@@ -1634,20 +1645,37 @@
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K32">
-    <sortCondition ref="A2:A32"/>
+  <sortState ref="A2:K33">
+    <sortCondition ref="A2:A33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1659,10 +1687,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1956,7 +1984,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>1</v>
@@ -1973,7 +2001,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>1</v>
@@ -1990,7 +2018,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>1</v>
@@ -2007,7 +2035,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>1</v>
@@ -2024,7 +2052,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>1</v>
@@ -2041,7 +2069,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>1</v>
@@ -2058,7 +2086,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>1</v>
@@ -2075,7 +2103,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>1</v>
@@ -2092,7 +2120,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>1</v>
@@ -2109,7 +2137,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>1</v>
@@ -2126,7 +2154,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>1</v>
@@ -2143,7 +2171,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>1</v>
@@ -2160,7 +2188,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>1</v>
@@ -2177,7 +2205,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>1</v>
@@ -2194,7 +2222,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>1</v>
@@ -2211,7 +2239,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>1</v>
@@ -2228,7 +2256,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>1</v>
@@ -2243,20 +2271,37 @@
       <c r="J32" s="16"/>
       <c r="K32" s="16"/>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K32">
-    <sortCondition ref="A2:A32"/>
+  <sortState ref="A2:K33">
+    <sortCondition ref="A2:A33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>